<commit_message>
updated test cases with global share value for login user
</commit_message>
<xml_diff>
--- a/SystemTest/SmokeSanityTestCases.xlsx
+++ b/SystemTest/SmokeSanityTestCases.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\svn\DanpheEMR\SystemTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\AutomationTest\SystemTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -96,9 +96,6 @@
     <t>TC007</t>
   </si>
   <si>
-    <t>Reports\TC004PatientCensusReport.py</t>
-  </si>
-  <si>
     <t>TC008</t>
   </si>
   <si>
@@ -123,12 +120,6 @@
     <t>TC012</t>
   </si>
   <si>
-    <t>EMR-2576</t>
-  </si>
-  <si>
-    <t>EMR-2547</t>
-  </si>
-  <si>
     <t>Norun</t>
   </si>
   <si>
@@ -147,9 +138,6 @@
     <t>TC014</t>
   </si>
   <si>
-    <t>TC015</t>
-  </si>
-  <si>
     <t>TC016</t>
   </si>
   <si>
@@ -160,9 +148,6 @@
   </si>
   <si>
     <t>TC019</t>
-  </si>
-  <si>
-    <t>EMR-2765, EMR-2766</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -180,7 +165,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -252,6 +237,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -526,15 +516,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -551,7 +542,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -560,7 +551,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -568,7 +559,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -587,7 +578,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -603,10 +594,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -625,7 +616,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -644,7 +635,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -663,7 +654,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -679,10 +670,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -693,12 +684,10 @@
       <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -706,7 +695,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
@@ -715,11 +704,9 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -727,7 +714,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
@@ -736,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -746,7 +733,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
@@ -755,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -765,7 +752,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
@@ -774,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -784,7 +771,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
@@ -793,17 +780,17 @@
         <v>0</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
@@ -812,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -822,7 +809,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
@@ -831,17 +818,17 @@
         <v>0</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -850,17 +837,17 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -869,17 +856,17 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
@@ -888,17 +875,17 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>18</v>
@@ -907,34 +894,13 @@
         <v>0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mass update for bulk test script execution
</commit_message>
<xml_diff>
--- a/SystemTest/SmokeSanityTestCases.xlsx
+++ b/SystemTest/SmokeSanityTestCases.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationGIT\SystemTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Automation\AutomationTest\SystemTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24450" yWindow="0" windowWidth="13905" windowHeight="12300"/>
+    <workbookView xWindow="25392" yWindow="0" windowWidth="13908" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -45,12 +45,6 @@
     <t>TC001</t>
   </si>
   <si>
-    <t>Patient\TC001PatientRegistrationPrintHealthCard.py</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
     <t>TC003</t>
   </si>
   <si>
@@ -66,60 +60,9 @@
     <t>TC005</t>
   </si>
   <si>
-    <t>Pharmacy\TC003PharmacyOPDbilling.py</t>
-  </si>
-  <si>
     <t>TC006</t>
   </si>
   <si>
-    <t>ADT\TC009AdmissionDischargeTransferToBeRefund.py</t>
-  </si>
-  <si>
-    <t>SanityTest</t>
-  </si>
-  <si>
-    <t>ADT\TC011AdmissionDischargeTransferNoDeposit.py</t>
-  </si>
-  <si>
-    <t>Nursing\TC001WardBilling&amp;AddVitals.py</t>
-  </si>
-  <si>
-    <t>Appointment\TC002CreateAppointmentFollowup.py</t>
-  </si>
-  <si>
-    <t>Reports\TC001BillingDashboardSummary.py</t>
-  </si>
-  <si>
-    <t>Reports\TC003SalesDayBookReport.py</t>
-  </si>
-  <si>
-    <t>TC007</t>
-  </si>
-  <si>
-    <t>TC008</t>
-  </si>
-  <si>
-    <t>Reports\TC005IncomeSegregationReport.py</t>
-  </si>
-  <si>
-    <t>TC009</t>
-  </si>
-  <si>
-    <t>Reports\TC006PatientCreditSummaryReport.py</t>
-  </si>
-  <si>
-    <t>TC010</t>
-  </si>
-  <si>
-    <t>Reports\TC007DoctorSummaryReport.py</t>
-  </si>
-  <si>
-    <t>TC011</t>
-  </si>
-  <si>
-    <t>TC012</t>
-  </si>
-  <si>
     <t>Norun</t>
   </si>
   <si>
@@ -129,52 +72,16 @@
     <t>Manual Status</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\TC010VerifyPharmacyDashboard.py</t>
-  </si>
-  <si>
-    <t>TC013</t>
-  </si>
-  <si>
-    <t>TC014</t>
-  </si>
-  <si>
-    <t>TC016</t>
-  </si>
-  <si>
-    <t>TC017</t>
-  </si>
-  <si>
-    <t>TC018</t>
-  </si>
-  <si>
-    <t>TC019</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Inventory\TC001CreateGoodReceipt.py</t>
-  </si>
-  <si>
-    <t>Billing\Opbilling\TC002OPDbillingLabXray.py</t>
-  </si>
-  <si>
-    <t>Billing\OPbilling\TC012CreateCopyOfItemsCreditInvoice.py</t>
-  </si>
-  <si>
-    <t>Deprecated: LPH</t>
-  </si>
-  <si>
-    <t>Hidden: LPH</t>
-  </si>
-  <si>
-    <t>OnHold: LPH</t>
+    <t>Billing\OPbilling\TC002OPDbillingLabXray.py</t>
+  </si>
+  <si>
+    <t>Dispensary\TC001CreateDispensarySale.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -525,22 +432,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" customWidth="1"/>
+    <col min="1" max="1" width="54.5546875" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -560,15 +467,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -582,12 +489,12 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -596,17 +503,17 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -620,12 +527,12 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -639,12 +546,12 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -653,270 +560,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="J8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>